<commit_message>
update de la feuille de temps et correction d'une erreur dans le content matrix
</commit_message>
<xml_diff>
--- a/Document/ContentMatrix_v1.5.xlsx
+++ b/Document/ContentMatrix_v1.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1257837\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1322931\Desktop\SERVIDER\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="241">
   <si>
     <t>VERSION</t>
   </si>
@@ -744,6 +744,12 @@
   </si>
   <si>
     <t xml:space="preserve">bouton publier </t>
+  </si>
+  <si>
+    <t>[Publish an Offer]</t>
+  </si>
+  <si>
+    <t>[Publier une annonce]</t>
   </si>
 </sst>
 </file>
@@ -753,11 +759,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1233,43 +1246,43 @@
   </borders>
   <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1299,25 +1312,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1326,13 +1339,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1341,121 +1354,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1464,37 +1477,37 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1506,73 +1519,73 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1584,32 +1597,35 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="31"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="31"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="32">
@@ -2239,9 +2255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R857"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2382,8 +2398,12 @@
       </c>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
+      <c r="J3" s="117" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" s="117" t="s">
+        <v>240</v>
+      </c>
       <c r="L3" s="60"/>
       <c r="M3" s="60"/>
       <c r="N3" s="60"/>
@@ -20436,12 +20456,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003DF93D1C80BCE4439E37126069156F2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac6bdae7674316788986ea2d0cdff43d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -20490,6 +20504,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -20500,20 +20520,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA27FEB7-001F-49B4-9822-FC9222977738}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20528,6 +20534,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
   <ds:schemaRefs>

</xml_diff>